<commit_message>
Logistica->Distribucion->Numero Guia Carga Masiva de Importes Fleteras Terminado
Pendiente agregar boton para crear y un boton para eliminar manual mente los importes
</commit_message>
<xml_diff>
--- a/public/templates/Template_Importes_NumeroGuia.xlsx
+++ b/public/templates/Template_Importes_NumeroGuia.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IndarRepositorys\PlataformaComercial\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0B85484-F8D0-4197-B901-CD0C6F0B9DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C273D1-201E-4500-ABEB-8E6D3F19D002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7704135F-3B7E-4942-96FD-6F2E55597E7B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="importes" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>